<commit_message>
Revert "Merge branch 'main' of https://github.com/kazarach/mitraaccounting"
This reverts commit c0db84661fc4af6cb097e5df81870fe8f9daf475, reversing
changes made to c94bc24c2c576d3028aeb96b5ee762c9931c75fb.
</commit_message>
<xml_diff>
--- a/FE JUAN.xlsx
+++ b/FE JUAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Juan\Project\mitraaccounting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\Mitra\mitraaccounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5392A8-9F15-4BA7-B930-30D96C3D989D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777448C1-5742-4AF9-9D1B-C21D52D91DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="30960" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,6 +54,9 @@
     <t>Pesanan Penjualan</t>
   </si>
   <si>
+    <t xml:space="preserve">Modal : category, supplier. </t>
+  </si>
+  <si>
     <t>Return Penjualan</t>
   </si>
   <si>
@@ -142,9 +145,6 @@
   </si>
   <si>
     <t>Barcode, Code, no Faktur, Tanggal, Nama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter Modal : category, supplier. </t>
   </si>
 </sst>
 </file>
@@ -160,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,12 +170,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,10 +186,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,17 +472,12 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,175 +488,171 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
       <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>